<commit_message>
Evaluate HS for different cases
And unmet demand / wasted surplus
</commit_message>
<xml_diff>
--- a/model/Inputs/model_inputs_elas.xlsx
+++ b/model/Inputs/model_inputs_elas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF8FE545-D04D-4C14-9F6B-16B5A40EFD3A}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5B75917-366F-4B52-976A-0088C0A62273}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -209,8 +209,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -268,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -284,6 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,8 +845,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +891,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="B2">
         <v>0.11</v>
@@ -1052,7 +1054,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,7 +1065,7 @@
     <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1129,7 +1131,7 @@
         <v>21.8</v>
       </c>
       <c r="G3">
-        <v>1.38E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1143,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5">
         <v>352</v>
@@ -1151,8 +1153,8 @@
       <c r="F4" s="5">
         <v>60.8</v>
       </c>
-      <c r="G4" s="5">
-        <v>0.6</v>
+      <c r="G4" s="7">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1374,8 +1376,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1390,7 +1392,7 @@
         <v>36</v>
       </c>
       <c r="B2">
-        <v>91</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1398,7 +1400,7 @@
         <v>37</v>
       </c>
       <c r="B3">
-        <v>153</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1406,7 +1408,7 @@
         <v>38</v>
       </c>
       <c r="B4">
-        <v>121</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1420,7 +1422,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B3" sqref="B3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,49 +1525,49 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>4.0201005025125598E-3</v>
       </c>
       <c r="H2">
-        <v>2.5819672131147539E-2</v>
+        <v>4.1170854271356763E-2</v>
       </c>
       <c r="I2">
-        <v>0.16275409836065571</v>
+        <v>0.15498492462311561</v>
       </c>
       <c r="J2">
-        <v>0.37470491803278688</v>
+        <v>0.34120100502512568</v>
       </c>
       <c r="K2">
-        <v>0.5609016393442624</v>
+        <v>0.51137185929648243</v>
       </c>
       <c r="L2">
-        <v>0.69518032786885242</v>
+        <v>0.63440201005025132</v>
       </c>
       <c r="M2">
-        <v>0.77686065573770491</v>
+        <v>0.70589447236180902</v>
       </c>
       <c r="N2">
-        <v>0.81105737704918035</v>
+        <v>0.7173165829145729</v>
       </c>
       <c r="O2">
-        <v>0.7935245901639344</v>
+        <v>0.67734170854271358</v>
       </c>
       <c r="P2">
-        <v>0.72468852459016386</v>
+        <v>0.57809547738693468</v>
       </c>
       <c r="Q2">
-        <v>0.60230327868852451</v>
+        <v>0.43412562814070349</v>
       </c>
       <c r="R2">
-        <v>0.43349180327868853</v>
+        <v>0.25252763819095481</v>
       </c>
       <c r="S2">
-        <v>0.23055737704918031</v>
+        <v>9.1608040201005048E-2</v>
       </c>
       <c r="T2">
-        <v>5.0016393442622951E-2</v>
+        <v>1.7597989949748739E-2</v>
       </c>
       <c r="U2">
-        <v>2.991803278688524E-3</v>
+        <v>3.2160804020100472E-4</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1600,49 +1602,49 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>2.1509433962264152E-3</v>
       </c>
       <c r="H3">
-        <v>1.335294117647059E-2</v>
+        <v>2.0773584905660381E-2</v>
       </c>
       <c r="I3">
-        <v>0.1510457516339869</v>
+        <v>7.4056603773584917E-2</v>
       </c>
       <c r="J3">
-        <v>0.36648366013071898</v>
+        <v>0.20321698113207551</v>
       </c>
       <c r="K3">
-        <v>0.54676470588235293</v>
+        <v>0.34733018867924531</v>
       </c>
       <c r="L3">
-        <v>0.66818954248366014</v>
+        <v>0.46702830188679251</v>
       </c>
       <c r="M3">
-        <v>0.73162745098039206</v>
+        <v>0.54499999999999993</v>
       </c>
       <c r="N3">
-        <v>0.74206535947712415</v>
+        <v>0.55942452830188683</v>
       </c>
       <c r="O3">
-        <v>0.70073202614379082</v>
+        <v>0.51176415094339622</v>
       </c>
       <c r="P3">
-        <v>0.59535947712418302</v>
+        <v>0.41073584905660382</v>
       </c>
       <c r="Q3">
-        <v>0.43600653594771238</v>
+        <v>0.27456603773584909</v>
       </c>
       <c r="R3">
-        <v>0.24354901960784309</v>
+        <v>0.13354716981132081</v>
       </c>
       <c r="S3">
-        <v>0.11178431372549021</v>
+        <v>3.995283018867922E-2</v>
       </c>
       <c r="T3">
-        <v>1.822875816993464E-2</v>
+        <v>8.6698113207547139E-3</v>
       </c>
       <c r="U3">
-        <v>4.3790849673202621E-4</v>
+        <v>1.4150943396226421E-4</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1677,49 +1679,49 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>4.3956043956043948E-5</v>
+        <v>1.8032786885245899E-3</v>
       </c>
       <c r="H4">
-        <v>3.9714285714285723E-2</v>
+        <v>1.6032786885245912E-2</v>
       </c>
       <c r="I4">
-        <v>0.1988681318681319</v>
+        <v>5.4229508196721322E-2</v>
       </c>
       <c r="J4">
-        <v>0.3788791208791209</v>
+        <v>0.1274918032786885</v>
       </c>
       <c r="K4">
-        <v>0.52748351648351643</v>
+        <v>0.20950819672131141</v>
       </c>
       <c r="L4">
-        <v>0.62382417582417582</v>
+        <v>0.26809836065573772</v>
       </c>
       <c r="M4">
-        <v>0.66321978021978023</v>
+        <v>0.28267213114754092</v>
       </c>
       <c r="N4">
-        <v>0.6375384615384615</v>
+        <v>0.27595081967213131</v>
       </c>
       <c r="O4">
-        <v>0.55946153846153845</v>
+        <v>0.25488524590163941</v>
       </c>
       <c r="P4">
-        <v>0.43716483516483517</v>
+        <v>0.21809836065573759</v>
       </c>
       <c r="Q4">
-        <v>0.26671428571428568</v>
+        <v>0.151</v>
       </c>
       <c r="R4">
-        <v>8.4153846153846162E-2</v>
+        <v>8.1081967213114725E-2</v>
       </c>
       <c r="S4">
-        <v>4.6263736263736262E-3</v>
+        <v>3.1426229508196707E-2</v>
       </c>
       <c r="T4">
-        <v>2.5274725274725281E-4</v>
+        <v>7.7049180327868824E-3</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>9.8360655737705021E-5</v>
       </c>
       <c r="V4">
         <v>0</v>

</xml_diff>

<commit_message>
Fix excess battery usage bug
</commit_message>
<xml_diff>
--- a/model/Inputs/model_inputs_elas.xlsx
+++ b/model/Inputs/model_inputs_elas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5B75917-366F-4B52-976A-0088C0A62273}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172BCDA7-6190-4AE1-8E83-098B4C7581AC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1408,7 +1408,7 @@
         <v>38</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2600,11 +2600,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2861,27 +2862,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2906,9 +2897,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>